<commit_message>
Updating Projects to Include Graduate Courses
</commit_message>
<xml_diff>
--- a/NEABrazil/Excel Analysis.xlsx
+++ b/NEABrazil/Excel Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a6c8dc3d867d216b/Desktop/PersonalProjects/NEABrazil/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjone\OneDrive\Desktop\PersonalProjects\NEABrazil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4F27F968-A775-46A4-9CBC-FB923EA1F836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{4F27F968-A775-46A4-9CBC-FB923EA1F836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF8D3CF6-34C9-49CD-997D-F1DE0DCC63C5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,12 +22,12 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="71" r:id="rId7"/>
-    <pivotCache cacheId="74" r:id="rId8"/>
-    <pivotCache cacheId="77" r:id="rId9"/>
-    <pivotCache cacheId="81" r:id="rId10"/>
-    <pivotCache cacheId="84" r:id="rId11"/>
-    <pivotCache cacheId="87" r:id="rId12"/>
+    <pivotCache cacheId="12" r:id="rId7"/>
+    <pivotCache cacheId="13" r:id="rId8"/>
+    <pivotCache cacheId="14" r:id="rId9"/>
+    <pivotCache cacheId="15" r:id="rId10"/>
+    <pivotCache cacheId="16" r:id="rId11"/>
+    <pivotCache cacheId="17" r:id="rId12"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -889,12 +889,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -940,69 +934,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1018,7 +949,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1049,13 +979,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1086,7 +1009,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1098,6 +1020,54 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1123,45 +1093,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1340,6 +1271,9 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -1347,9 +1281,168 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -1519,12 +1612,201 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1619,13 +1901,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
@@ -1635,282 +1910,7 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -2803,6 +2803,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2859,6 +2862,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2915,6 +2921,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2971,6 +2980,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3027,6 +3039,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3083,6 +3098,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4279,6 +4297,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4335,6 +4356,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4391,6 +4415,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -9804,14 +9831,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>998220</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1897380</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2743200</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
@@ -9842,7 +9869,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391390972225" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391390972225" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5" xr:uid="{00000000-000A-0000-FFFF-FFFF47000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table13"/>
   </cacheSource>
@@ -9878,7 +9905,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391390972225" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391390972225" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5" xr:uid="{00000000-000A-0000-FFFF-FFFF4A000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table12"/>
   </cacheSource>
@@ -9911,7 +9938,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391390972225" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391390972225" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5" xr:uid="{00000000-000A-0000-FFFF-FFFF4D000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table9"/>
   </cacheSource>
@@ -9944,7 +9971,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391391087964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="36">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391391087964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="36" xr:uid="{00000000-000A-0000-FFFF-FFFF51000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -9997,7 +10024,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391391087964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391391087964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5" xr:uid="{00000000-000A-0000-FFFF-FFFF54000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table14"/>
   </cacheSource>
@@ -10030,7 +10057,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391391087964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Megan Jones" refreshedDate="43764.391391087964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5" xr:uid="{00000000-000A-0000-FFFF-FFFF57000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table15"/>
   </cacheSource>
@@ -10572,7 +10599,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="81" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A4:F6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -10707,7 +10734,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable9" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="E21:H27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -10808,7 +10835,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="77" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A12:B18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -10878,7 +10905,77 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="84" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable5" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="A22:B28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Inflation, GDP deflator (annual %)" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable7" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="F22:I28" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -10978,78 +11075,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="74" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="A22:B28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="44" showAll="0"/>
-    <pivotField numFmtId="44" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Inflation, GDP deflator (annual %)" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="71" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable6" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="F19:J25" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -11164,68 +11191,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:I4" totalsRowShown="0">
-  <autoFilter ref="A1:I4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="A1:I4" totalsRowShown="0">
+  <autoFilter ref="A1:I4" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Country Name"/>
-    <tableColumn id="2" name="Country Code"/>
-    <tableColumn id="3" name="Series Name"/>
-    <tableColumn id="4" name="Series Code"/>
-    <tableColumn id="5" name="2014"/>
-    <tableColumn id="6" name="2015"/>
-    <tableColumn id="7" name="2016"/>
-    <tableColumn id="8" name="2017"/>
-    <tableColumn id="9" name="2018"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Country Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Country Code"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Series Name"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Series Code"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="2014"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="2015"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="2016"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="2017"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2018"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G13" totalsRowShown="0" headerRowDxfId="34" dataDxfId="35" headerRowBorderDxfId="44" tableBorderDxfId="45" totalsRowBorderDxfId="43">
-  <autoFilter ref="A1:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table2" displayName="Table2" ref="A1:G13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:G13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Country Name" dataDxfId="42"/>
-    <tableColumn id="2" name="Series Name" dataDxfId="41"/>
-    <tableColumn id="3" name="2014" dataDxfId="40"/>
-    <tableColumn id="4" name="2015" dataDxfId="39"/>
-    <tableColumn id="5" name="2016" dataDxfId="38"/>
-    <tableColumn id="6" name="2017" dataDxfId="37"/>
-    <tableColumn id="7" name="2018" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Country Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Series Name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="2014" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="2015" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="2016" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="2017" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="2018" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A6:D11" totalsRowShown="0" headerRowBorderDxfId="32" tableBorderDxfId="33" totalsRowBorderDxfId="31">
-  <autoFilter ref="A6:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table9" displayName="Table9" ref="A6:D11" totalsRowShown="0" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="A6:D11" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Year" dataDxfId="30"/>
-    <tableColumn id="2" name="GDP (current US$)" dataDxfId="29" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="GDP growth (annual %)" dataDxfId="0"/>
-    <tableColumn id="4" name="GDP per capita (current US$)" dataDxfId="28" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Year" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="GDP (current US$)" dataDxfId="41" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="GDP growth (annual %)" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="GDP per capita (current US$)" dataDxfId="39" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="E13:H18" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="E13:H18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table15" displayName="Table15" ref="E13:H18" totalsRowShown="0" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="E13:H18" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Year" dataDxfId="4"/>
-    <tableColumn id="2" name="Brazil" dataDxfId="3"/>
-    <tableColumn id="3" name="World" dataDxfId="2"/>
-    <tableColumn id="4" name="United States" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Year" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Brazil" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="World" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="United States" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table112" displayName="Table112" ref="A1:G10" totalsRowShown="0">
-  <autoFilter ref="A1:G10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table112" displayName="Table112" ref="A1:G10" totalsRowShown="0">
+  <autoFilter ref="A1:G10" xr:uid="{00000000-0009-0000-0100-00000B000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="Brazil"/>
@@ -11236,47 +11263,47 @@
     <sortCondition ref="B1:B7"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Country Name"/>
-    <tableColumn id="3" name="Series Name"/>
-    <tableColumn id="5" name="2014"/>
-    <tableColumn id="6" name="2015"/>
-    <tableColumn id="7" name="2016"/>
-    <tableColumn id="8" name="2017"/>
-    <tableColumn id="9" name="2018"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Country Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Series Name"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="2014"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="2015"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="2016"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="2017"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="2018"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A14:D19" totalsRowShown="0" tableBorderDxfId="27">
-  <autoFilter ref="A14:D19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table12" displayName="Table12" ref="A14:D19" totalsRowShown="0" tableBorderDxfId="31">
+  <autoFilter ref="A14:D19" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="YEAR" dataDxfId="26"/>
-    <tableColumn id="2" name="GNI (current US$)" dataDxfId="25" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="GNI per capita (constant 2010 US$)" dataDxfId="24" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="Inflation, GDP deflator (annual %)" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="YEAR" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="GNI (current US$)" dataDxfId="29" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="GNI per capita (constant 2010 US$)" dataDxfId="28" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Inflation, GDP deflator (annual %)" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="F15:I20" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
-  <autoFilter ref="F15:I20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table14" displayName="Table14" ref="F15:I20" totalsRowShown="0" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="F15:I20" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="YEAR" dataDxfId="11"/>
-    <tableColumn id="2" name="Brazil" dataDxfId="10" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="World" dataDxfId="9" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="United States" dataDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="YEAR" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Brazil" dataDxfId="22" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="World" dataDxfId="21" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="United States" dataDxfId="20" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table111" displayName="Table111" ref="A1:G16" totalsRowShown="0">
-  <autoFilter ref="A1:G16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table111" displayName="Table111" ref="A1:G16" totalsRowShown="0">
+  <autoFilter ref="A1:G16" xr:uid="{00000000-0009-0000-0100-00000A000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="Brazil"/>
@@ -11287,46 +11314,46 @@
     <sortCondition ref="B1:B16"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Country Name"/>
-    <tableColumn id="3" name="Series Name"/>
-    <tableColumn id="5" name="2014"/>
-    <tableColumn id="6" name="2015"/>
-    <tableColumn id="7" name="2016"/>
-    <tableColumn id="8" name="2017"/>
-    <tableColumn id="9" name="2018"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Country Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Series Name"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="2014"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="2015"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="2016"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="2017"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="2018"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A22:E27" totalsRowShown="0" headerRowBorderDxfId="21" tableBorderDxfId="22" totalsRowBorderDxfId="20">
-  <autoFilter ref="A22:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A22:E27" totalsRowShown="0" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A22:E27" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Year" dataDxfId="19"/>
-    <tableColumn id="2" name="Unemployment with advanced education (% of total labor force with advanced education)" dataDxfId="18"/>
-    <tableColumn id="3" name="Unemployment with basic education (% of total labor force with basic education)" dataDxfId="17"/>
-    <tableColumn id="4" name="Unemployment with intermediate education (% of total labor force with intermediate education)" dataDxfId="16"/>
-    <tableColumn id="5" name="Unemployment, total (% of total labor force) (modeled ILO estimate)" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Year" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Unemployment with advanced education (% of total labor force with advanced education)" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Unemployment with basic education (% of total labor force with basic education)" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Unemployment with intermediate education (% of total labor force with intermediate education)" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Unemployment, total (% of total labor force) (modeled ILO estimate)" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G37" totalsRowShown="0">
-  <autoFilter ref="A1:G37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table1" displayName="Table1" ref="A1:G37" totalsRowShown="0">
+  <autoFilter ref="A1:G37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G37">
     <sortCondition ref="B1:B37"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Country Name"/>
-    <tableColumn id="3" name="Series Name"/>
-    <tableColumn id="5" name="2014"/>
-    <tableColumn id="6" name="2015"/>
-    <tableColumn id="7" name="2016"/>
-    <tableColumn id="8" name="2017"/>
-    <tableColumn id="9" name="2018"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Country Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Series Name"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="2014"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="2015"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="2016"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="2017"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="2018"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11628,7 +11655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11717,7 +11744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12177,7 +12204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12845,11 +12872,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13513,7 +13540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
@@ -14398,7 +14425,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>